<commit_message>
Update code according to POM
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Content_Testing_LeapFrog-games.xlsx
+++ b/src/test/resources/data/Content_Testing_LeapFrog-games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin's\OneDrive\Máy tính\Sele3\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0BDFB6-106F-49E6-89AC-EB852A73F850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AF8B46-7AC2-42D8-B17D-2756707A0CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{F15A1851-A1FC-4588-BC0C-29CC66F8709B}"/>
   </bookViews>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update log for allure report
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Content_Testing_LeapFrog-games.xlsx
+++ b/src/test/resources/data/Content_Testing_LeapFrog-games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin's\OneDrive\Máy tính\Sele3\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AF8B46-7AC2-42D8-B17D-2756707A0CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7494354C-84A9-48E0-8B49-810A01DDB7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{F15A1851-A1FC-4588-BC0C-29CC66F8709B}"/>
   </bookViews>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Push code to review
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Content_Testing_LeapFrog-games.xlsx
+++ b/src/test/resources/data/Content_Testing_LeapFrog-games.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin's\OneDrive\Máy tính\Sele3\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thai.luu\Desktop\Sele3\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7494354C-84A9-48E0-8B49-810A01DDB7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{F15A1851-A1FC-4588-BC0C-29CC66F8709B}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="26295" windowHeight="14175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>title</t>
   </si>
@@ -59,9 +58,6 @@
     <t>4-8 years</t>
   </si>
   <si>
-    <t>(French) Football : Championnat des maths</t>
-  </si>
-  <si>
     <t>(French) L'alphabet en cuisine</t>
   </si>
   <si>
@@ -78,9 +74,6 @@
   </si>
   <si>
     <t>(Spanish) Bob Esponja Tesoros del Mar</t>
-  </si>
-  <si>
-    <t>7-12 years</t>
   </si>
   <si>
     <t>(Spanish) Disney Princesas: Canciones de l...</t>
@@ -148,7 +141,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -158,7 +151,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -183,30 +176,39 @@
   <si>
     <t>(French) Copains canins – Mes amis les chiens !</t>
   </si>
+  <si>
+    <t>(French) Football : Khampionnat des maths</t>
+  </si>
+  <si>
+    <t>7-15 years</t>
+  </si>
+  <si>
+    <t>$11.00</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -214,7 +216,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -222,7 +224,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -230,35 +232,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -266,7 +268,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -274,14 +276,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -289,14 +291,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -304,7 +306,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -312,14 +314,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -327,7 +329,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -674,9 +676,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1052,69 +1055,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2F211C-9048-4846-96DF-9A13FA16ADB0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15">
+      <c r="B7" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{D556F603-7B46-42E0-A023-80F6A366BA2E}"/>
+    <hyperlink ref="B1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8987AF49-65DD-4180-9D2D-DBD25824F5FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1125,9 +1128,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1136,9 +1139,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1147,9 +1150,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1158,9 +1161,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1169,20 +1172,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1191,20 +1194,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1213,31 +1216,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1246,9 +1249,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -1257,9 +1260,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1268,31 +1271,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -1301,9 +1304,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1312,9 +1315,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1323,20 +1326,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -1345,20 +1348,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -1367,9 +1370,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -1378,9 +1381,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>

</xml_diff>